<commit_message>
Remove some comments + add script to test laser tokenizer
</commit_message>
<xml_diff>
--- a/Results_merged.xlsx
+++ b/Results_merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Univer\3_kurs\Comparison_of_methods_for_multilingual_semantic_search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C45F7A-D06D-49D1-BC1C-C79F4D950462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0843CB-253B-43C7-B193-430C4C52EE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7710" yWindow="3615" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="32">
   <si>
     <t>model</t>
   </si>
@@ -133,12 +133,27 @@
   <si>
     <t>LASER (FLatL2)</t>
   </si>
+  <si>
+    <t>Rezultāti rakstu nosaukumu tekstiem</t>
+  </si>
+  <si>
+    <t>Rezultāti rakstu ievadu tekstiem</t>
+  </si>
+  <si>
+    <t>Rezultāti rakstu pilnājiem tekstiem</t>
+  </si>
+  <si>
+    <t>mBERT</t>
+  </si>
+  <si>
+    <t>rezultātu uzlabojums palielinot K no 1 līdz 10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +188,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF595959"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -187,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -219,20 +241,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -240,7 +293,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -294,64 +371,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Rezultāti rakstu nosaukumu tekstiem</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.1353575775573469E-2"/>
+          <c:y val="7.9110423198768876E-2"/>
+          <c:w val="0.91186421620000835"/>
+          <c:h val="0.82536038241394349"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -379,7 +411,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -448,7 +490,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="plus"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -517,7 +569,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -587,7 +649,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
@@ -639,7 +711,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
@@ -691,7 +773,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
@@ -726,6 +818,917 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1236183456"/>
+        <c:axId val="1236170016"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1236183456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="lv-LV" sz="1200">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>k</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1236170016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1236170016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="lv-LV" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Pārklājums, %</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1236183456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.1268123806359593E-2"/>
+          <c:y val="7.9110423198768876E-2"/>
+          <c:w val="0.91196976628915327"/>
+          <c:h val="0.84197481226425452"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mBERT (HNSW)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$39:$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$46:$F$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7ECC-455B-AA9B-12BCCD26E06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>XLM-RoBERTa (HNSW)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="plus"/>
+              <c:size val="7"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-7ECC-455B-AA9B-12BCCD26E06C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="plus"/>
+              <c:size val="7"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent5"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-7ECC-455B-AA9B-12BCCD26E06C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$39:$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$47:$F$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7ECC-455B-AA9B-12BCCD26E06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LASER (HNSW)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$39:$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$48:$F$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9.07</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.93</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7ECC-455B-AA9B-12BCCD26E06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mBERT (FLatL2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$39:$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$46:$M$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7ECC-455B-AA9B-12BCCD26E06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>XLM-RoBERTa (FLatL2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$39:$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$47:$M$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.58</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-7ECC-455B-AA9B-12BCCD26E06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LASER (FLatL2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$39:$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$48:$M$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-7ECC-455B-AA9B-12BCCD26E06C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1236183456"/>
         <c:axId val="1236170016"/>
@@ -888,7 +1891,7 @@
                     <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
-                  <a:t>Pārklājums</a:t>
+                  <a:t>Pārklājums, %</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="1200">
                   <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -970,8 +1973,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
+      <c:legendPos val="r"/>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1044,7 +2047,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1058,72 +2061,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Rezultāti </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="lv-LV"/>
-              <a:t>rakstu ievadu </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>tekstiem</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.1682239888971017E-2"/>
+          <c:y val="7.6977491864210545E-2"/>
+          <c:w val="0.91145825099186895"/>
+          <c:h val="0.79007554349037357"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1151,7 +2101,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1192,7 +2152,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7FA5-4B64-9D96-5C4116219A40}"/>
+              <c16:uniqueId val="{00000000-0565-4D1B-B586-1679EA3965EC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1220,7 +2180,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="plus"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1261,7 +2231,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7FA5-4B64-9D96-5C4116219A40}"/>
+              <c16:uniqueId val="{00000001-0565-4D1B-B586-1679EA3965EC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1289,7 +2259,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1330,7 +2310,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7FA5-4B64-9D96-5C4116219A40}"/>
+              <c16:uniqueId val="{00000002-0565-4D1B-B586-1679EA3965EC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1359,7 +2339,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1400,7 +2390,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-7FA5-4B64-9D96-5C4116219A40}"/>
+              <c16:uniqueId val="{00000003-0565-4D1B-B586-1679EA3965EC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1429,7 +2419,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1470,7 +2470,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-7FA5-4B64-9D96-5C4116219A40}"/>
+              <c16:uniqueId val="{00000004-0565-4D1B-B586-1679EA3965EC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1499,7 +2499,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1540,7 +2550,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-7FA5-4B64-9D96-5C4116219A40}"/>
+              <c16:uniqueId val="{00000005-0565-4D1B-B586-1679EA3965EC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1552,6 +2562,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1236183456"/>
         <c:axId val="1236170016"/>
@@ -1696,13 +2707,27 @@
               <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      </a:sysClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1710,13 +2735,25 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="lv-LV" sz="1200">
+                  <a:rPr lang="lv-LV" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
                     <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
-                  <a:t>Pārklājums</a:t>
+                  <a:t>Pārklājums, %</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1200">
+                <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
                   <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:endParaRPr>
@@ -1735,13 +2772,27 @@
             <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
+                    <a:sysClr val="windowText" lastClr="000000">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    </a:sysClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1796,880 +2847,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Rezultāti </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="lv-LV"/>
-              <a:t>rakstu pilnājiem</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="lv-LV" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>tekstiem</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$34</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>mBERT (HNSW)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$39:$F$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$46:$F$46</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.18</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.57999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.86</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7ECC-455B-AA9B-12BCCD26E06C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>XLM-RoBERTa (HNSW)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:marker>
-              <c:symbol val="none"/>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-7ECC-455B-AA9B-12BCCD26E06C}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="none"/>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="28575" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-7ECC-455B-AA9B-12BCCD26E06C}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$39:$F$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$47:$F$47</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.09</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7ECC-455B-AA9B-12BCCD26E06C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$36</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>LASER (HNSW)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$39:$F$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$48:$F$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>9.07</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.93</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7ECC-455B-AA9B-12BCCD26E06C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$J$34</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>mBERT (FLatL2)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$39:$F$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$K$46:$M$46</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.19</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.91</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-7ECC-455B-AA9B-12BCCD26E06C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$J$35</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>XLM-RoBERTa (FLatL2)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$39:$F$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$K$47:$M$47</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.58</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.66</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.08</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-7ECC-455B-AA9B-12BCCD26E06C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$J$36</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>LASER (FLatL2)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$D$39:$F$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$K$48:$M$48</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>10.23</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.66</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.18</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-7ECC-455B-AA9B-12BCCD26E06C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1236183456"/>
-        <c:axId val="1236170016"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1236183456"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="lv-LV" sz="1200">
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:rPr>
-                  <a:t>k</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1200">
-                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                </a:endParaRPr>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1236170016"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1236170016"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="lv-LV" sz="1200">
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:rPr>
-                  <a:t>Pārklājums</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1200">
-                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                </a:endParaRPr>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1236183456"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
+      <c:legendPos val="r"/>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4417,13 +4596,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>187696</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>30815</xdr:rowOff>
+      <xdr:rowOff>30816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1676400</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>79562</xdr:rowOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>123266</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4450,23 +4629,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>827</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>598714</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>166895</xdr:rowOff>
+      <xdr:rowOff>176894</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>579029</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>25142</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>470647</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>100854</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="20" name="Chart 19">
+        <xdr:cNvPr id="21" name="Chart 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F7A49EB-9405-404E-8D65-48B6150530CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA2AC48-4F1A-4CE4-876A-CCA5509D339D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4488,23 +4667,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>598714</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>122145</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>16809</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>360487</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>35140</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>95229</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>116</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="21" name="Chart 20">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA2AC48-4F1A-4CE4-876A-CCA5509D339D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A623BF66-103E-4358-978A-EF2AEE0D0F8C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4561,13 +4740,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41395D38-1EFA-4BB9-9669-3BBC694E4B3C}" name="Results_HNSW" displayName="Results_HNSW" ref="A2:G29" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A2:G29" xr:uid="{41395D38-1EFA-4BB9-9669-3BBC694E4B3C}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="source"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:G29" xr:uid="{41395D38-1EFA-4BB9-9669-3BBC694E4B3C}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{AB76D40D-A4D9-4C2C-9026-224770AEC22E}" uniqueName="1" name="model" queryTableFieldId="1" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{94CC2946-3B9C-43D9-AB5C-219A2F93E9D1}" uniqueName="2" name="type" queryTableFieldId="2" dataDxfId="4"/>
@@ -4860,10 +5033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O49"/>
+  <dimension ref="A1:AK83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y39" sqref="Y39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W35" sqref="W35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4881,27 +5054,29 @@
     <col min="13" max="13" width="13.7109375" customWidth="1"/>
     <col min="14" max="14" width="13.42578125" customWidth="1"/>
     <col min="15" max="15" width="6.85546875" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="21" max="21" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4947,7 +5122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -4991,7 +5166,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5035,7 +5210,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -5211,7 +5386,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5255,7 +5430,7 @@
         <v>15.56</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -5299,7 +5474,7 @@
         <v>17.52</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -5343,7 +5518,7 @@
         <v>18.579999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -5387,7 +5562,7 @@
         <v>29.98</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -5431,7 +5606,7 @@
         <v>38.590000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -5563,7 +5738,7 @@
         <v>13.66</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -5607,7 +5782,7 @@
         <v>15.18</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -5651,7 +5826,7 @@
         <v>46.09</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -5695,7 +5870,7 @@
         <v>53.68</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -5739,7 +5914,7 @@
         <v>56.01</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -5783,7 +5958,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -5827,7 +6002,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -5871,7 +6046,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -5915,7 +6090,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -5959,7 +6134,7 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -6003,7 +6178,7 @@
         <v>5.08</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -6047,7 +6222,7 @@
         <v>14.67</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -6091,7 +6266,7 @@
         <v>16.72</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -6135,524 +6310,730 @@
         <v>17.68</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
+    <row r="30" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="U30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+    </row>
+    <row r="31" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
       <c r="C31" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="2"/>
-      <c r="I31" s="2"/>
+      <c r="G31" s="1"/>
+      <c r="I31" s="1"/>
       <c r="J31" s="7" t="s">
         <v>17</v>
       </c>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
-      <c r="N31" s="2"/>
+      <c r="N31" s="1"/>
+      <c r="U31" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V31" s="12"/>
+      <c r="W31" s="12"/>
+      <c r="X31" s="12"/>
+      <c r="Y31" s="13"/>
     </row>
-    <row r="32" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="3" t="s">
+    <row r="32" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="3" t="s">
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="2"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="1"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X32" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y32" s="13"/>
     </row>
-    <row r="33" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="4">
+    <row r="33" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="2">
         <v>1</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="2">
         <v>5</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="2">
         <v>10</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="4">
+      <c r="G33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="2">
         <v>1</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33" s="2">
         <v>5</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M33" s="2">
         <v>10</v>
       </c>
-      <c r="N33" s="2"/>
+      <c r="N33" s="1"/>
+      <c r="U33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V33" s="4">
+        <f>M34-K34</f>
+        <v>3.0199999999999978</v>
+      </c>
+      <c r="W33" s="4">
+        <f>M40-K40</f>
+        <v>0.19</v>
+      </c>
+      <c r="X33" s="8">
+        <f>M46-K46</f>
+        <v>0.72</v>
+      </c>
+      <c r="Y33" s="9"/>
     </row>
-    <row r="34" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="C34" s="4" t="s">
+    <row r="34" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+      <c r="C34" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="4">
         <f>$G$9</f>
         <v>15.21</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="4">
         <f>$G$10</f>
         <v>16.899999999999999</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="4">
         <f>$G$11</f>
         <v>17.690000000000001</v>
       </c>
-      <c r="G34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="4" t="s">
+      <c r="G34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K34" s="6">
+      <c r="K34" s="4">
         <f>$O$9</f>
         <v>15.56</v>
       </c>
-      <c r="L34" s="6">
+      <c r="L34" s="4">
         <f>$O$10</f>
         <v>17.52</v>
       </c>
-      <c r="M34" s="6">
+      <c r="M34" s="4">
         <f>$O$11</f>
         <v>18.579999999999998</v>
       </c>
-      <c r="N34" s="2"/>
+      <c r="N34" s="1"/>
+      <c r="U34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V34" s="4">
+        <f>M35-K35</f>
+        <v>3.01</v>
+      </c>
+      <c r="W34" s="4">
+        <f t="shared" ref="W34:W35" si="0">M41-K41</f>
+        <v>0.26</v>
+      </c>
+      <c r="X34" s="8">
+        <f t="shared" ref="X34:X35" si="1">M47-K47</f>
+        <v>3.5</v>
+      </c>
+      <c r="Y34" s="9"/>
     </row>
-    <row r="35" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="C35" s="4" t="s">
+    <row r="35" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="C35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="4">
         <f>$G$27</f>
         <v>14.1</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="4">
         <f>$G$28</f>
         <v>15.79</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="4">
         <f>$G$29</f>
         <v>16.52</v>
       </c>
-      <c r="G35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="4" t="s">
+      <c r="G35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K35" s="6">
+      <c r="K35" s="4">
         <f>$O$27</f>
         <v>14.67</v>
       </c>
-      <c r="L35" s="6">
+      <c r="L35" s="4">
         <f>$O$28</f>
         <v>16.72</v>
       </c>
-      <c r="M35" s="6">
+      <c r="M35" s="4">
         <f>$O$29</f>
         <v>17.68</v>
       </c>
-      <c r="N35" s="2"/>
+      <c r="N35" s="1"/>
+      <c r="U35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V35" s="4">
+        <f>M36-K36</f>
+        <v>9.9199999999999946</v>
+      </c>
+      <c r="W35" s="4">
+        <f t="shared" si="0"/>
+        <v>12.34</v>
+      </c>
+      <c r="X35" s="8">
+        <f t="shared" si="1"/>
+        <v>4.9499999999999993</v>
+      </c>
+      <c r="Y35" s="9"/>
     </row>
-    <row r="36" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="C36" s="4" t="s">
+    <row r="36" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="C36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="4">
         <f>$G$18</f>
         <v>43.14</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="4">
         <f>$G$19</f>
         <v>49.19</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="4">
         <f>$G$20</f>
         <v>50.82</v>
       </c>
-      <c r="G36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="4" t="s">
+      <c r="G36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K36" s="6">
+      <c r="K36" s="4">
         <f>$O$18</f>
         <v>46.09</v>
       </c>
-      <c r="L36" s="6">
+      <c r="L36" s="4">
         <f>$O$19</f>
         <v>53.68</v>
       </c>
-      <c r="M36" s="6">
+      <c r="M36" s="4">
         <f>$O$20</f>
         <v>56.01</v>
       </c>
-      <c r="N36" s="2"/>
+      <c r="N36" s="1"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
     </row>
-    <row r="38" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
-      <c r="C38" s="3" t="s">
+    <row r="38" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="3" t="s">
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="2"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="1"/>
+      <c r="U38" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
     </row>
-    <row r="39" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="4">
+    <row r="39" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="2">
         <v>1</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="2">
         <v>5</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="2">
         <v>10</v>
       </c>
-      <c r="G39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="4">
+      <c r="G39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="2">
         <v>1</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39" s="2">
         <v>5</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M39" s="2">
         <v>10</v>
       </c>
-      <c r="N39" s="2"/>
+      <c r="N39" s="1"/>
+      <c r="U39" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V39" s="12"/>
+      <c r="W39" s="12"/>
+      <c r="X39" s="12"/>
+      <c r="Y39" s="13"/>
     </row>
-    <row r="40" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
-      <c r="C40" s="4" t="s">
+    <row r="40" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="C40" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="4">
         <f>$G$3</f>
         <v>0.03</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="4">
         <f>$G$4</f>
         <v>0.12</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="4">
         <f>$G$5</f>
         <v>0.22</v>
       </c>
-      <c r="G40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="4" t="s">
+      <c r="G40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K40" s="6">
+      <c r="K40" s="4">
         <f>$O$3</f>
         <v>0.03</v>
       </c>
-      <c r="L40" s="6">
+      <c r="L40" s="4">
         <f>$O$4</f>
         <v>0.13</v>
       </c>
-      <c r="M40" s="6">
+      <c r="M40" s="4">
         <f>$O$5</f>
         <v>0.22</v>
       </c>
-      <c r="N40" s="2"/>
+      <c r="N40" s="1"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="W40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X40" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y40" s="13"/>
     </row>
-    <row r="41" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
-      <c r="C41" s="4" t="s">
+    <row r="41" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="C41" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="4">
         <f>$G$21</f>
         <v>0.03</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="4">
         <f>$G$22</f>
         <v>0.16</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="4">
         <f>$G$23</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="G41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="4" t="s">
+      <c r="G41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K41" s="6">
+      <c r="K41" s="4">
         <f>$O$21</f>
         <v>0.03</v>
       </c>
-      <c r="L41" s="6">
+      <c r="L41" s="4">
         <f>$O$22</f>
         <v>0.17</v>
       </c>
-      <c r="M41" s="6">
+      <c r="M41" s="4">
         <f>$O$23</f>
         <v>0.28999999999999998</v>
       </c>
-      <c r="N41" s="2"/>
+      <c r="N41" s="1"/>
+      <c r="U41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V41" s="4">
+        <f>F34-D34</f>
+        <v>2.4800000000000004</v>
+      </c>
+      <c r="W41" s="4">
+        <f>F40-D40</f>
+        <v>0.19</v>
+      </c>
+      <c r="X41" s="8">
+        <f>F46-D46</f>
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="Y41" s="9"/>
     </row>
-    <row r="42" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
-      <c r="C42" s="4" t="s">
+    <row r="42" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="C42" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="4">
         <f>$G$12</f>
         <v>26.11</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="4">
         <f>$G$13</f>
         <v>32.75</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42" s="4">
         <f>$G$14</f>
         <v>35.4</v>
       </c>
-      <c r="G42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="4" t="s">
+      <c r="G42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K42" s="6">
+      <c r="K42" s="4">
         <f>$O$12</f>
         <v>29.98</v>
       </c>
-      <c r="L42" s="6">
+      <c r="L42" s="4">
         <f>$O$13</f>
         <v>38.590000000000003</v>
       </c>
-      <c r="M42" s="6">
+      <c r="M42" s="4">
         <f>$O$14</f>
         <v>42.32</v>
       </c>
-      <c r="N42" s="2"/>
+      <c r="N42" s="1"/>
+      <c r="U42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V42" s="4">
+        <f t="shared" ref="V42:V43" si="2">F35-D35</f>
+        <v>2.42</v>
+      </c>
+      <c r="W42" s="4">
+        <f t="shared" ref="W42:W43" si="3">F41-D41</f>
+        <v>0.25</v>
+      </c>
+      <c r="X42" s="8">
+        <f t="shared" ref="X42:X43" si="4">F47-D47</f>
+        <v>2.8699999999999997</v>
+      </c>
+      <c r="Y42" s="9"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
+    <row r="43" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="U43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V43" s="4">
+        <f t="shared" si="2"/>
+        <v>7.68</v>
+      </c>
+      <c r="W43" s="4">
+        <f t="shared" si="3"/>
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="X43" s="8">
+        <f t="shared" si="4"/>
+        <v>4.0299999999999994</v>
+      </c>
+      <c r="Y43" s="9"/>
     </row>
-    <row r="44" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
-      <c r="C44" s="3" t="s">
+    <row r="44" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+      <c r="C44" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="3" t="s">
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="2"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="4">
+    <row r="45" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="2">
         <v>1</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="2">
         <v>5</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45" s="2">
         <v>10</v>
       </c>
-      <c r="G45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="4">
+      <c r="G45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="2">
         <v>1</v>
       </c>
-      <c r="L45" s="4">
+      <c r="L45" s="2">
         <v>5</v>
       </c>
-      <c r="M45" s="4">
+      <c r="M45" s="2">
         <v>10</v>
       </c>
-      <c r="N45" s="2"/>
+      <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
-      <c r="C46" s="4" t="s">
+    <row r="46" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+      <c r="C46" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="4">
         <f>$G$6</f>
         <v>0.18</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="4">
         <f>$G$7</f>
         <v>0.57999999999999996</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="4">
         <f>$G$8</f>
         <v>0.86</v>
       </c>
-      <c r="G46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="4" t="s">
+      <c r="G46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K46" s="6">
+      <c r="K46" s="4">
         <f>$O$6</f>
         <v>0.19</v>
       </c>
-      <c r="L46" s="6">
+      <c r="L46" s="4">
         <f>$O$7</f>
         <v>0.6</v>
       </c>
-      <c r="M46" s="6">
+      <c r="M46" s="4">
         <f>$O$8</f>
         <v>0.91</v>
       </c>
-      <c r="N46" s="2"/>
+      <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-      <c r="C47" s="4" t="s">
+    <row r="47" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+      <c r="C47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="4">
         <f>$G$24</f>
         <v>1.35</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="4">
         <f>$G$25</f>
         <v>3.09</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="4">
         <f>$G$26</f>
         <v>4.22</v>
       </c>
-      <c r="G47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="4" t="s">
+      <c r="G47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K47" s="6">
+      <c r="K47" s="4">
         <f>$O$24</f>
         <v>1.58</v>
       </c>
-      <c r="L47" s="6">
+      <c r="L47" s="4">
         <f>$O$25</f>
         <v>3.66</v>
       </c>
-      <c r="M47" s="6">
+      <c r="M47" s="4">
         <f>$O$26</f>
         <v>5.08</v>
       </c>
-      <c r="N47" s="2"/>
+      <c r="N47" s="1"/>
     </row>
-    <row r="48" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
-      <c r="C48" s="4" t="s">
+    <row r="48" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+      <c r="C48" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="4">
         <f>$G$15</f>
         <v>9.07</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="4">
         <f>$G$16</f>
         <v>11.93</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="4">
         <f>$G$17</f>
         <v>13.1</v>
       </c>
-      <c r="G48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="4" t="s">
+      <c r="G48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K48" s="6">
+      <c r="K48" s="4">
         <f>$O$15</f>
         <v>10.23</v>
       </c>
-      <c r="L48" s="6">
+      <c r="L48" s="4">
         <f>$O$16</f>
         <v>13.66</v>
       </c>
-      <c r="M48" s="6">
+      <c r="M48" s="4">
         <f>$O$17</f>
         <v>15.18</v>
       </c>
-      <c r="N48" s="2"/>
+      <c r="N48" s="1"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+    </row>
+    <row r="83" spans="3:37" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C83" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="10"/>
+      <c r="L83" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M83" s="10"/>
+      <c r="N83" s="10"/>
+      <c r="O83" s="10"/>
+      <c r="P83" s="10"/>
+      <c r="Q83" s="10"/>
+      <c r="R83" s="10"/>
+      <c r="S83" s="10"/>
+      <c r="T83" s="10"/>
+      <c r="U83" s="10"/>
+      <c r="V83" s="10"/>
+      <c r="W83" s="10"/>
+      <c r="Y83" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z83" s="10"/>
+      <c r="AA83" s="10"/>
+      <c r="AB83" s="10"/>
+      <c r="AC83" s="10"/>
+      <c r="AD83" s="10"/>
+      <c r="AE83" s="10"/>
+      <c r="AF83" s="10"/>
+      <c r="AG83" s="10"/>
+      <c r="AH83" s="10"/>
+      <c r="AI83" s="10"/>
+      <c r="AJ83" s="10"/>
+      <c r="AK83" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="25">
+    <mergeCell ref="X33:Y33"/>
+    <mergeCell ref="X34:Y34"/>
+    <mergeCell ref="X35:Y35"/>
+    <mergeCell ref="U30:Y30"/>
+    <mergeCell ref="C83:J83"/>
+    <mergeCell ref="L83:W83"/>
+    <mergeCell ref="Y83:AK83"/>
+    <mergeCell ref="U31:Y31"/>
+    <mergeCell ref="X32:Y32"/>
+    <mergeCell ref="X43:Y43"/>
+    <mergeCell ref="U38:Y38"/>
+    <mergeCell ref="U39:Y39"/>
+    <mergeCell ref="X40:Y40"/>
+    <mergeCell ref="X41:Y41"/>
+    <mergeCell ref="X42:Y42"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:O1"/>
     <mergeCell ref="C44:F44"/>
     <mergeCell ref="J32:M32"/>
     <mergeCell ref="J38:M38"/>
@@ -6661,8 +7042,6 @@
     <mergeCell ref="J31:M31"/>
     <mergeCell ref="C32:F32"/>
     <mergeCell ref="C38:F38"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="I1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>